<commit_message>
Adding dictonaries and list of products and branches. Remaking coding lines
</commit_message>
<xml_diff>
--- a/archivos/1-Pedido LARPI2.xlsx
+++ b/archivos/1-Pedido LARPI2.xlsx
@@ -1070,510 +1070,1706 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="A20" t="n">
+        <v>51</v>
+      </c>
+      <c r="B20" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>2320060000009</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AKUSAY X KG      </t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="A21" t="n">
+        <v>51</v>
+      </c>
+      <c r="B21" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>2320061000008</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA CAPUCHINA X KG      </t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
+      <c r="A22" t="n">
+        <v>51</v>
+      </c>
+      <c r="B22" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>2320062000007</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA CRIOLLA x kg.      </t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
+      <c r="A23" t="n">
+        <v>51</v>
+      </c>
+      <c r="B23" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>2320065000004</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HINOJO X KG.      </t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+      <c r="A24" t="n">
+        <v>51</v>
+      </c>
+      <c r="B24" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>2320066000003</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA FRANCESA X KG.      </t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="A25" t="n">
+        <v>51</v>
+      </c>
+      <c r="B25" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>2320067000002</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA MANTECOSA X KG.      </t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="A26" t="n">
+        <v>51</v>
+      </c>
+      <c r="B26" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>2320071000005</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">APIO X KG.      </t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
+      <c r="A27" t="n">
+        <v>51</v>
+      </c>
+      <c r="B27" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>2320073000003</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO BLANCO x kg.-      </t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+      <c r="A28" t="n">
+        <v>51</v>
+      </c>
+      <c r="B28" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>2320074000002</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO COLORADO X KG.      </t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="A29" t="n">
+        <v>51</v>
+      </c>
+      <c r="B29" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>2320076000000</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BROCOLI x kg.      </t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+      <c r="A30" t="n">
+        <v>51</v>
+      </c>
+      <c r="B30" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>2320078000008</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COLIFLOR x kg.      </t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
+      <c r="A31" t="n">
+        <v>51</v>
+      </c>
+      <c r="B31" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>2920176200005</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ACELGA X PAQUETE      </t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
+      <c r="A32" t="n">
+        <v>51</v>
+      </c>
+      <c r="B32" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>2920176600003</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CEBOLLA DE VERDEO X ATADO      </t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+      <c r="A33" t="n">
+        <v>51</v>
+      </c>
+      <c r="B33" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>2920176800007</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESPINACA X ATADO      </t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="A34" t="n">
+        <v>51</v>
+      </c>
+      <c r="B34" t="n">
+        <v>282154</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>2920176900004</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PEREJIL X ATADO      </t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
+      <c r="A35" t="n">
+        <v>118</v>
+      </c>
+      <c r="B35" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>2320061000008</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA CAPUCHINA X KG      </t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+      <c r="A36" t="n">
+        <v>118</v>
+      </c>
+      <c r="B36" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>2320062000007</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA CRIOLLA x kg.      </t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+      <c r="A37" t="n">
+        <v>118</v>
+      </c>
+      <c r="B37" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>2320066000003</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA FRANCESA X KG.      </t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
+      <c r="A38" t="n">
+        <v>118</v>
+      </c>
+      <c r="B38" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>2320067000002</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA MANTECOSA X KG.      </t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+      <c r="A39" t="n">
+        <v>118</v>
+      </c>
+      <c r="B39" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>2320071000005</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">APIO X KG.      </t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+      <c r="A40" t="n">
+        <v>118</v>
+      </c>
+      <c r="B40" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>2320073000003</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO BLANCO x kg.-      </t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
+      <c r="A41" t="n">
+        <v>118</v>
+      </c>
+      <c r="B41" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>2320076000000</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BROCOLI x kg.      </t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
+      <c r="A42" t="n">
+        <v>118</v>
+      </c>
+      <c r="B42" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>2320078000008</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COLIFLOR x kg.      </t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
+      <c r="A43" t="n">
+        <v>118</v>
+      </c>
+      <c r="B43" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>2320095000005</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REMOLACHA X KG.      </t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
+      <c r="A44" t="n">
+        <v>118</v>
+      </c>
+      <c r="B44" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>2920176200005</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ACELGA X PAQUETE      </t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
+      <c r="A45" t="n">
+        <v>118</v>
+      </c>
+      <c r="B45" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>2920176600003</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CEBOLLA DE VERDEO X ATADO      </t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="A46" t="n">
+        <v>118</v>
+      </c>
+      <c r="B46" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>2920176800007</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESPINACA X ATADO      </t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
+      <c r="A47" t="n">
+        <v>118</v>
+      </c>
+      <c r="B47" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>2920176900004</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PEREJIL X ATADO      </t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
+      <c r="A48" t="n">
+        <v>118</v>
+      </c>
+      <c r="B48" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>2920177000000</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUERRO X ATADO      </t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
+      <c r="A49" t="n">
+        <v>118</v>
+      </c>
+      <c r="B49" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>2920177100007</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RABANITO X ATADO.      </t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
+      <c r="A50" t="n">
+        <v>118</v>
+      </c>
+      <c r="B50" t="n">
+        <v>334569</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>2920177200004</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RUCULA X ATADO      </t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
+      <c r="A51" t="n">
+        <v>150</v>
+      </c>
+      <c r="B51" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>2320061000008</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA CAPUCHINA X KG      </t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
+      <c r="A52" t="n">
+        <v>150</v>
+      </c>
+      <c r="B52" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>2320062000007</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA CRIOLLA x kg.      </t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
+      <c r="A53" t="n">
+        <v>150</v>
+      </c>
+      <c r="B53" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>2320063000006</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA ESCAROLA X KG      </t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
+      <c r="A54" t="n">
+        <v>150</v>
+      </c>
+      <c r="B54" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>2320066000003</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA FRANCESA X KG.      </t>
+        </is>
+      </c>
+      <c r="I54" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
+      <c r="A55" t="n">
+        <v>150</v>
+      </c>
+      <c r="B55" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>2320067000002</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LECHUGA MANTECOSA X KG.      </t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="A56" t="n">
+        <v>150</v>
+      </c>
+      <c r="B56" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>2320071000005</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">APIO X KG.      </t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
+      <c r="A57" t="n">
+        <v>150</v>
+      </c>
+      <c r="B57" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>2320073000003</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO BLANCO x kg.-      </t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr"/>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+      <c r="A58" t="n">
+        <v>150</v>
+      </c>
+      <c r="B58" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>2320074000002</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO COLORADO X KG.      </t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+      <c r="A59" t="n">
+        <v>150</v>
+      </c>
+      <c r="B59" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>2320076000000</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BROCOLI x kg.      </t>
+        </is>
+      </c>
+      <c r="I59" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
+      <c r="A60" t="n">
+        <v>150</v>
+      </c>
+      <c r="B60" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>2320078000008</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COLIFLOR x kg.      </t>
+        </is>
+      </c>
+      <c r="I60" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr"/>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
+      <c r="A61" t="n">
+        <v>150</v>
+      </c>
+      <c r="B61" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>2920176200005</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ACELGA X PAQUETE      </t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr"/>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
+      <c r="A62" t="n">
+        <v>150</v>
+      </c>
+      <c r="B62" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D62" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>2920176600003</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CEBOLLA DE VERDEO X ATADO      </t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr"/>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
+      <c r="A63" t="n">
+        <v>150</v>
+      </c>
+      <c r="B63" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>2920176800007</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESPINACA X ATADO      </t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr"/>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
+      <c r="A64" t="n">
+        <v>150</v>
+      </c>
+      <c r="B64" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D64" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>2920176900004</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PEREJIL X ATADO      </t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr"/>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
+      <c r="A65" t="n">
+        <v>150</v>
+      </c>
+      <c r="B65" t="n">
+        <v>291588</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>CONF</t>
+        </is>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2022-06-10</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>2920177000000</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUERRO X ATADO      </t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr"/>
@@ -2366,6 +3562,512 @@
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="inlineStr"/>
       <c r="I137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr"/>
+      <c r="F138" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr"/>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr"/>
+      <c r="I141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="inlineStr"/>
+      <c r="F145" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr"/>
+      <c r="F148" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr"/>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="inlineStr"/>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr"/>
+      <c r="I155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="inlineStr"/>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr"/>
+      <c r="I156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr"/>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr"/>
+      <c r="I157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr"/>
+      <c r="I158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="inlineStr"/>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr"/>
+      <c r="I159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr"/>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr"/>
+      <c r="I160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr"/>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="inlineStr"/>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr"/>
+      <c r="I161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr"/>
+      <c r="I162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr"/>
+      <c r="B163" t="inlineStr"/>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr"/>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr"/>
+      <c r="F164" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr"/>
+      <c r="B165" t="inlineStr"/>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr"/>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr"/>
+      <c r="B167" t="inlineStr"/>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr"/>
+      <c r="F167" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr"/>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr"/>
+      <c r="F168" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr"/>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr"/>
+      <c r="B170" t="inlineStr"/>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr"/>
+      <c r="F170" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr"/>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="inlineStr"/>
+      <c r="F171" t="inlineStr"/>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" t="inlineStr"/>
+      <c r="I171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="inlineStr"/>
+      <c r="F172" t="inlineStr"/>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" t="inlineStr"/>
+      <c r="I172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="inlineStr"/>
+      <c r="D173" t="inlineStr"/>
+      <c r="E173" t="inlineStr"/>
+      <c r="F173" t="inlineStr"/>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" t="inlineStr"/>
+      <c r="I173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="inlineStr"/>
+      <c r="D174" t="inlineStr"/>
+      <c r="E174" t="inlineStr"/>
+      <c r="F174" t="inlineStr"/>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" t="inlineStr"/>
+      <c r="I174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="inlineStr"/>
+      <c r="D175" t="inlineStr"/>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" t="inlineStr"/>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" t="inlineStr"/>
+      <c r="I175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr"/>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="inlineStr"/>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" t="inlineStr"/>
+      <c r="I176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="inlineStr"/>
+      <c r="F177" t="inlineStr"/>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" t="inlineStr"/>
+      <c r="I177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr"/>
+      <c r="C178" t="inlineStr"/>
+      <c r="D178" t="inlineStr"/>
+      <c r="E178" t="inlineStr"/>
+      <c r="F178" t="inlineStr"/>
+      <c r="G178" t="inlineStr"/>
+      <c r="H178" t="inlineStr"/>
+      <c r="I178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr"/>
+      <c r="C179" t="inlineStr"/>
+      <c r="D179" t="inlineStr"/>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" t="inlineStr"/>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" t="inlineStr"/>
+      <c r="I179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr"/>
+      <c r="C180" t="inlineStr"/>
+      <c r="D180" t="inlineStr"/>
+      <c r="E180" t="inlineStr"/>
+      <c r="F180" t="inlineStr"/>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" t="inlineStr"/>
+      <c r="I180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr"/>
+      <c r="C181" t="inlineStr"/>
+      <c r="D181" t="inlineStr"/>
+      <c r="E181" t="inlineStr"/>
+      <c r="F181" t="inlineStr"/>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" t="inlineStr"/>
+      <c r="I181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" t="inlineStr"/>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr"/>
+      <c r="I182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
+      <c r="E183" t="inlineStr"/>
+      <c r="F183" t="inlineStr"/>
+      <c r="G183" t="inlineStr"/>
+      <c r="H183" t="inlineStr"/>
+      <c r="I183" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>